<commit_message>
Exception handling mechanism added
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="24">
   <si>
     <t>testname</t>
   </si>
@@ -78,6 +78,15 @@
   </si>
   <si>
     <t>chrome</t>
+  </si>
+  <si>
+    <t>amazonPageTest</t>
+  </si>
+  <si>
+    <t>Amazon-Page-Test</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -431,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,7 +483,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>7</v>
@@ -488,12 +497,29 @@
         <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -505,10 +531,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,7 +591,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -585,7 +611,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
@@ -625,7 +651,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
@@ -637,6 +663,26 @@
         <v>15</v>
       </c>
       <c r="F6" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>